<commit_message>
fix: Resolve device initialization and management issues
- Fix device initialization failure due to id_1 index duplicate key error
- Remove automatic initDevices call on server restart to prevent redundant updates
- Plan manual init-devices API and frontend button for admin control
- Fix /devices/manage route to render DeviceManage.jsx instead of DevicesSubMenu
- Resolve syntax error in App.jsx around line 54 (closing braces and export)
- Enable device registration on /devices/manage with proper CORS credentials
- Add debugging logs for better request/response tracking
</commit_message>
<xml_diff>
--- a/backend/device-data.xlsx
+++ b/backend/device-data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28619"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28627"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22CA3816-928F-49A4-8241-F8D995A2E151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEBF2A89-5289-4822-A350-C21715137891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,46 +31,71 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+  <si>
+    <t>SerialNumber</t>
   </si>
   <si>
     <t>DeviceInfo</t>
   </si>
   <si>
-    <t>Category</t>
+    <t>OSName</t>
   </si>
   <si>
     <t>OSVersion</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Device123</t>
-  </si>
-  <si>
-    <t>Game</t>
-  </si>
-  <si>
-    <t>Tokyo</t>
+    <t>ModelName</t>
+  </si>
+  <si>
+    <t>GD_A_001</t>
+  </si>
+  <si>
+    <t>갤럭시</t>
+  </si>
+  <si>
+    <t>AOS</t>
+  </si>
+  <si>
+    <t>GD_A_002</t>
+  </si>
+  <si>
+    <t>GD_A_003</t>
+  </si>
+  <si>
+    <t>GD_A_004</t>
+  </si>
+  <si>
+    <t>GD_A_005</t>
+  </si>
+  <si>
+    <t>GD_i_001</t>
+  </si>
+  <si>
+    <t>아이폰</t>
+  </si>
+  <si>
+    <t>iOS</t>
+  </si>
+  <si>
+    <t>GD_i_002</t>
+  </si>
+  <si>
+    <t>GD_i_003</t>
+  </si>
+  <si>
+    <t>GD_i_004</t>
+  </si>
+  <si>
+    <t>GD_i_005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -100,7 +125,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -435,48 +462,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>